<commit_message>
update data ke desember 2025, update notebook dan dashboard mesin
</commit_message>
<xml_diff>
--- a/raw_data/R098 Kediri/2024_01_Transaksi Paket Kartu Summary Berdasarkan Tipe Kartu dan Paket Kartu.xlsx
+++ b/raw_data/R098 Kediri/2024_01_Transaksi Paket Kartu Summary Berdasarkan Tipe Kartu dan Paket Kartu.xlsx
@@ -23,7 +23,7 @@
     </r>
   </si>
   <si>
-    <t>03042</t>
+    <t>08008</t>
   </si>
   <si>
     <r>
@@ -31,7 +31,7 @@
     </r>
   </si>
   <si>
-    <t>Sabar Subur</t>
+    <t>Kediri (R-98)</t>
   </si>
   <si>
     <r>
@@ -50,6 +50,9 @@
     <r>
       <t>Center:</t>
     </r>
+  </si>
+  <si>
+    <t>Kediri (R-98) RMS</t>
   </si>
   <si>
     <r>
@@ -106,16 +109,10 @@
     </r>
   </si>
   <si>
-    <t>JUMAT-MINGGU  KIDIELAND 1 JAM</t>
+    <t>KDL BARU 20K</t>
   </si>
   <si>
-    <t>JUMAT-MINGGU KIDIELAND SEPUASNYA</t>
-  </si>
-  <si>
-    <t>SENIN-KAMIS KIDIELAND 1 JAM</t>
-  </si>
-  <si>
-    <t>SENIN-KAMIS SEPUASNYA KIDIELAND</t>
+    <t>KDL ISI ULANG  20K</t>
   </si>
   <si>
     <r>
@@ -126,43 +123,94 @@
     <t>Zone</t>
   </si>
   <si>
-    <t>BONUS SALDO JUARA 1</t>
+    <t>ISI ULANG MIN 10K S/D 49K</t>
   </si>
   <si>
-    <t>BONUS SALDO JUARA 2</t>
+    <t>KARTU BARU Rp 30.000</t>
   </si>
   <si>
-    <t>BONUS SALDO JUARA 3</t>
+    <t>KARTU BARU Rp 50.000</t>
   </si>
   <si>
-    <t>FREE GAME</t>
+    <t>PAKET 100K + 50% + (POPCRON+CIDEA)</t>
   </si>
   <si>
-    <t>Isi Ulang Zone Rp.2 Rb s/d Rp.49 Rb</t>
+    <t>PAKET 100K + 50% + (POPCRON+ICE CREAM)</t>
   </si>
   <si>
-    <t>Isi Ulang Zone Rp.50 Rb s/d Rp.99 Rb</t>
+    <t>PAKET 100K + 50% + 1 cidea + 1 ice cream</t>
   </si>
   <si>
-    <t>PEMBELIAN 100K TEH BOTOL+FRUTTEA</t>
+    <t>PAKET 100K + 50% + 1 POPCRON + 1 CIDEA</t>
   </si>
   <si>
-    <t>PEMBELIAN 150 K PAKET NYEMIL C</t>
+    <t>PAKET 100K + 50% + 2 CIDEA</t>
   </si>
   <si>
-    <t>PEMBELIAN 3O K FREE GAME</t>
+    <t>PAKET 100K + 50% + 2 play cafe (20K)</t>
   </si>
   <si>
-    <t>PEMBELIAN 50 K</t>
+    <t>PAKET 100K + 50% + 2 play cafe (24K)</t>
   </si>
   <si>
-    <t>PEMBELIAN 50 K FRUTTEA</t>
+    <t>PAKET 100K + 50% + 2 POPCRON</t>
   </si>
   <si>
-    <t>PEMBELIAN 50 K TEH BOTOL</t>
+    <t>PAKET 100K + 50% + 2 POPCRON + KURSI PIJAT + KUPON</t>
   </si>
   <si>
-    <t>PROMO LOMBA MEWARNAI</t>
+    <t>PAKET 100K + 50% +1 POPCRON+1 CIDEA</t>
+  </si>
+  <si>
+    <t>PAKET 30K + 10% +  POPCRON</t>
+  </si>
+  <si>
+    <t>PAKET 30K + 10% + 1 play cafe (10K)</t>
+  </si>
+  <si>
+    <t>PAKET 30K + 10% + 1 play cafe (12K)</t>
+  </si>
+  <si>
+    <t>PAKET 30K + 10% +1 ice cream</t>
+  </si>
+  <si>
+    <t>PAKET 50K + 30% + 1 ice cream</t>
+  </si>
+  <si>
+    <t>PAKET 50K + 30% + 1 play cafe (10K)</t>
+  </si>
+  <si>
+    <t>PAKET 50K + 30% + 1 play cafe (12K)</t>
+  </si>
+  <si>
+    <t>PAKET 50K + 30% + 1 POPCRON</t>
+  </si>
+  <si>
+    <t>PAKET 50K + 30%+1CIDEA</t>
+  </si>
+  <si>
+    <t>PAKET 50K + 30%+1POPCRON</t>
+  </si>
+  <si>
+    <t>PAKET 50K + 30%+2POPCRON+KURSI PIJAT + KUPON JJ</t>
+  </si>
+  <si>
+    <t>PAKET 50K +30%+(POPCORN+CIDEA)</t>
+  </si>
+  <si>
+    <t>PAKET 50K +30%+(POPCORN+ICE CREAM)</t>
+  </si>
+  <si>
+    <t>PAKET 50K +30%+(POPCRON+CIDEA)</t>
+  </si>
+  <si>
+    <t>PAKET 50K +30%+(POPCRON+ICE CREAM)</t>
+  </si>
+  <si>
+    <t>PAKET KARTU MURAH PESERTA 5K BONUS 5K</t>
+  </si>
+  <si>
+    <t>SUPPORT LOMBA</t>
   </si>
   <si>
     <r>
@@ -399,7 +447,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:V46"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -16869,7 +16917,7 @@
       </c>
       <c r="S5" s="3"/>
       <c r="T5" s="5">
-        <v>46008</v>
+        <v>46030</v>
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -16886,7 +16934,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -16894,18 +16942,18 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="R6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="6">
-        <v>0.393043981481482</v>
+        <v>0.498923611111111</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
     </row>
     <row r="7" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7">
         <v>45292</v>
@@ -16917,7 +16965,7 @@
     </row>
     <row r="8" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7">
         <v>45322.9999884259</v>
@@ -16927,12 +16975,12 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="K8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -16945,7 +16993,7 @@
     <row r="9" ht="13.50" customHeight="1" outlineLevel="0"/>
     <row r="10" ht="15.75" customHeight="1" outlineLevel="0">
       <c r="A10" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -16971,12 +17019,12 @@
     </row>
     <row r="11" ht="10.50" customHeight="1" outlineLevel="0">
       <c r="I11" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" ht="12.00" customHeight="1" outlineLevel="0">
       <c r="A12" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -16986,20 +17034,20 @@
       <c r="G12" s="10"/>
       <c r="I12" s="9"/>
       <c r="J12" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K12" s="11"/>
       <c r="P12" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q12" s="9"/>
       <c r="R12" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S12" s="9"/>
       <c r="T12" s="9"/>
       <c r="U12" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V12" s="9"/>
     </row>
@@ -17023,7 +17071,7 @@
     </row>
     <row r="14" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A14" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -17032,18 +17080,18 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="I14" s="12">
-        <v>239</v>
+        <v>130</v>
       </c>
       <c r="J14" s="12">
-        <v>7170000</v>
+        <v>2600000</v>
       </c>
       <c r="K14" s="12"/>
       <c r="P14" s="12">
-        <v>478000</v>
+        <v>143000</v>
       </c>
       <c r="Q14" s="12"/>
       <c r="R14" s="12">
-        <v>6692000</v>
+        <v>2457000</v>
       </c>
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
@@ -17055,7 +17103,7 @@
     <row r="15" ht="10.50" customHeight="1" outlineLevel="0"/>
     <row r="16" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A16" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -17064,18 +17112,18 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="I16" s="12">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="J16" s="12">
-        <v>5145000</v>
+        <v>2260000</v>
       </c>
       <c r="K16" s="12"/>
       <c r="P16" s="12">
-        <v>0</v>
+        <v>124300</v>
       </c>
       <c r="Q16" s="12"/>
       <c r="R16" s="12">
-        <v>5145000</v>
+        <v>2135700</v>
       </c>
       <c r="S16" s="12"/>
       <c r="T16" s="12"/>
@@ -17085,175 +17133,145 @@
       <c r="V16" s="12"/>
     </row>
     <row r="17" ht="13.50" customHeight="1" outlineLevel="0">
-      <c r="A17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="I17" s="12">
-        <v>203</v>
-      </c>
-      <c r="J17" s="12">
-        <v>5405000</v>
-      </c>
-      <c r="K17" s="12"/>
-      <c r="P17" s="12">
-        <v>223000</v>
-      </c>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12">
-        <v>5182000</v>
-      </c>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12">
+      <c r="C17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="I17" s="14">
+        <v>243</v>
+      </c>
+      <c r="J17" s="14">
+        <v>4860000</v>
+      </c>
+      <c r="K17" s="14"/>
+      <c r="P17" s="14">
+        <v>267300</v>
+      </c>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14">
+        <v>4592700</v>
+      </c>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14">
         <v>0</v>
       </c>
-      <c r="V17" s="12"/>
+      <c r="V17" s="14"/>
     </row>
-    <row r="18" ht="13.50" customHeight="1" outlineLevel="0">
-      <c r="A18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="I18" s="12">
-        <v>126</v>
-      </c>
-      <c r="J18" s="12">
-        <v>4060000</v>
-      </c>
-      <c r="K18" s="12"/>
-      <c r="P18" s="12">
-        <v>112000</v>
-      </c>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12">
-        <v>3948000</v>
-      </c>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="12">
+    <row r="18" ht="12.75" customHeight="1" outlineLevel="0"/>
+    <row r="19" ht="15.75" customHeight="1" outlineLevel="0">
+      <c r="A19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+    </row>
+    <row r="20" ht="10.50" customHeight="1" outlineLevel="0">
+      <c r="I20" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" ht="12.00" customHeight="1" outlineLevel="0">
+      <c r="A21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="P21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="V21" s="9"/>
+    </row>
+    <row r="22" ht="1.50" customHeight="1" outlineLevel="0">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+    </row>
+    <row r="23" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="I23" s="12">
+        <v>11</v>
+      </c>
+      <c r="J23" s="12">
+        <v>195000</v>
+      </c>
+      <c r="K23" s="12"/>
+      <c r="P23" s="12">
         <v>0</v>
       </c>
-      <c r="V18" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12">
+        <v>195000</v>
+      </c>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12">
+        <v>0</v>
+      </c>
+      <c r="V23" s="12"/>
     </row>
-    <row r="19" ht="13.50" customHeight="1" outlineLevel="0">
-      <c r="C19" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="I19" s="14">
-        <v>715</v>
-      </c>
-      <c r="J19" s="14">
-        <v>21780000</v>
-      </c>
-      <c r="K19" s="14"/>
-      <c r="P19" s="14">
-        <v>813000</v>
-      </c>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14">
-        <v>20967000</v>
-      </c>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14">
-        <v>0</v>
-      </c>
-      <c r="V19" s="14"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1" outlineLevel="0"/>
-    <row r="21" ht="15.75" customHeight="1" outlineLevel="0">
-      <c r="A21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-    </row>
-    <row r="22" ht="10.50" customHeight="1" outlineLevel="0">
-      <c r="I22" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" ht="12.00" customHeight="1" outlineLevel="0">
-      <c r="A23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23" s="11"/>
-      <c r="P23" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="V23" s="9"/>
-    </row>
-    <row r="24" ht="1.50" customHeight="1" outlineLevel="0">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-    </row>
+    <row r="24" ht="10.50" customHeight="1" outlineLevel="0"/>
     <row r="25" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A25" s="4" t="s">
         <v>28</v>
@@ -17265,10 +17283,10 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="I25" s="12">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J25" s="12">
-        <v>0</v>
+        <v>540000</v>
       </c>
       <c r="K25" s="12"/>
       <c r="P25" s="12">
@@ -17276,19 +17294,49 @@
       </c>
       <c r="Q25" s="12"/>
       <c r="R25" s="12">
-        <v>0</v>
+        <v>540000</v>
       </c>
       <c r="S25" s="12"/>
       <c r="T25" s="12"/>
       <c r="U25" s="12">
-        <v>198800</v>
+        <v>0</v>
       </c>
       <c r="V25" s="12"/>
     </row>
-    <row r="26" ht="10.50" customHeight="1" outlineLevel="0"/>
+    <row r="26" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="I26" s="12">
+        <v>293</v>
+      </c>
+      <c r="J26" s="12">
+        <v>14650000</v>
+      </c>
+      <c r="K26" s="12"/>
+      <c r="P26" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12">
+        <v>14650000</v>
+      </c>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12">
+        <v>0</v>
+      </c>
+      <c r="V26" s="12"/>
+    </row>
     <row r="27" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A27" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -17300,7 +17348,7 @@
         <v>2</v>
       </c>
       <c r="J27" s="12">
-        <v>0</v>
+        <v>156000</v>
       </c>
       <c r="K27" s="12"/>
       <c r="P27" s="12">
@@ -17308,18 +17356,18 @@
       </c>
       <c r="Q27" s="12"/>
       <c r="R27" s="12">
-        <v>0</v>
+        <v>156000</v>
       </c>
       <c r="S27" s="12"/>
       <c r="T27" s="12"/>
       <c r="U27" s="12">
-        <v>149800</v>
+        <v>144200</v>
       </c>
       <c r="V27" s="12"/>
     </row>
     <row r="28" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A28" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -17328,10 +17376,10 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="I28" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J28" s="12">
-        <v>0</v>
+        <v>234000</v>
       </c>
       <c r="K28" s="12"/>
       <c r="P28" s="12">
@@ -17339,18 +17387,18 @@
       </c>
       <c r="Q28" s="12"/>
       <c r="R28" s="12">
-        <v>0</v>
+        <v>234000</v>
       </c>
       <c r="S28" s="12"/>
       <c r="T28" s="12"/>
       <c r="U28" s="12">
-        <v>99400</v>
+        <v>216300</v>
       </c>
       <c r="V28" s="12"/>
     </row>
     <row r="29" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A29" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -17359,10 +17407,10 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="I29" s="12">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="J29" s="12">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="K29" s="12"/>
       <c r="P29" s="12">
@@ -17370,18 +17418,18 @@
       </c>
       <c r="Q29" s="12"/>
       <c r="R29" s="12">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="S29" s="12"/>
       <c r="T29" s="12"/>
       <c r="U29" s="12">
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="V29" s="12"/>
     </row>
     <row r="30" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A30" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -17390,10 +17438,10 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="I30" s="12">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="J30" s="12">
-        <v>2895000</v>
+        <v>78000</v>
       </c>
       <c r="K30" s="12"/>
       <c r="P30" s="12">
@@ -17401,18 +17449,18 @@
       </c>
       <c r="Q30" s="12"/>
       <c r="R30" s="12">
-        <v>2895000</v>
+        <v>78000</v>
       </c>
       <c r="S30" s="12"/>
       <c r="T30" s="12"/>
       <c r="U30" s="12">
-        <v>0</v>
+        <v>72100</v>
       </c>
       <c r="V30" s="12"/>
     </row>
     <row r="31" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A31" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -17421,10 +17469,10 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="I31" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J31" s="12">
-        <v>50000</v>
+        <v>160000</v>
       </c>
       <c r="K31" s="12"/>
       <c r="P31" s="12">
@@ -17432,18 +17480,18 @@
       </c>
       <c r="Q31" s="12"/>
       <c r="R31" s="12">
-        <v>50000</v>
+        <v>160000</v>
       </c>
       <c r="S31" s="12"/>
       <c r="T31" s="12"/>
       <c r="U31" s="12">
-        <v>14700</v>
+        <v>140000</v>
       </c>
       <c r="V31" s="12"/>
     </row>
     <row r="32" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A32" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -17452,10 +17500,10 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="I32" s="12">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="J32" s="12">
-        <v>7462000</v>
+        <v>400000</v>
       </c>
       <c r="K32" s="12"/>
       <c r="P32" s="12">
@@ -17463,18 +17511,18 @@
       </c>
       <c r="Q32" s="12"/>
       <c r="R32" s="12">
-        <v>7462000</v>
+        <v>400000</v>
       </c>
       <c r="S32" s="12"/>
       <c r="T32" s="12"/>
       <c r="U32" s="12">
-        <v>4331600</v>
+        <v>350000</v>
       </c>
       <c r="V32" s="12"/>
     </row>
     <row r="33" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A33" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -17483,10 +17531,10 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="I33" s="12">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J33" s="12">
-        <v>805000</v>
+        <v>152000</v>
       </c>
       <c r="K33" s="12"/>
       <c r="P33" s="12">
@@ -17494,18 +17542,18 @@
       </c>
       <c r="Q33" s="12"/>
       <c r="R33" s="12">
-        <v>805000</v>
+        <v>152000</v>
       </c>
       <c r="S33" s="12"/>
       <c r="T33" s="12"/>
       <c r="U33" s="12">
-        <v>769300</v>
+        <v>147000</v>
       </c>
       <c r="V33" s="12"/>
     </row>
     <row r="34" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A34" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -17514,10 +17562,10 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="I34" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J34" s="12">
-        <v>60000</v>
+        <v>304000</v>
       </c>
       <c r="K34" s="12"/>
       <c r="P34" s="12">
@@ -17525,18 +17573,18 @@
       </c>
       <c r="Q34" s="12"/>
       <c r="R34" s="12">
-        <v>60000</v>
+        <v>304000</v>
       </c>
       <c r="S34" s="12"/>
       <c r="T34" s="12"/>
       <c r="U34" s="12">
-        <v>53200</v>
+        <v>296800</v>
       </c>
       <c r="V34" s="12"/>
     </row>
     <row r="35" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A35" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -17545,10 +17593,10 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="I35" s="12">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="J35" s="12">
-        <v>4100000</v>
+        <v>1064000</v>
       </c>
       <c r="K35" s="12"/>
       <c r="P35" s="12">
@@ -17556,18 +17604,18 @@
       </c>
       <c r="Q35" s="12"/>
       <c r="R35" s="12">
-        <v>4100000</v>
+        <v>1064000</v>
       </c>
       <c r="S35" s="12"/>
       <c r="T35" s="12"/>
       <c r="U35" s="12">
-        <v>459200</v>
+        <v>1048600</v>
       </c>
       <c r="V35" s="12"/>
     </row>
     <row r="36" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A36" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -17576,10 +17624,10 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="I36" s="12">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="J36" s="12">
-        <v>4346000</v>
+        <v>78000</v>
       </c>
       <c r="K36" s="12"/>
       <c r="P36" s="12">
@@ -17587,18 +17635,18 @@
       </c>
       <c r="Q36" s="12"/>
       <c r="R36" s="12">
-        <v>4346000</v>
+        <v>78000</v>
       </c>
       <c r="S36" s="12"/>
       <c r="T36" s="12"/>
       <c r="U36" s="12">
-        <v>1484000</v>
+        <v>72100</v>
       </c>
       <c r="V36" s="12"/>
     </row>
     <row r="37" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A37" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -17607,10 +17655,10 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="I37" s="12">
-        <v>198</v>
+        <v>75</v>
       </c>
       <c r="J37" s="12">
-        <v>8118000</v>
+        <v>1350000</v>
       </c>
       <c r="K37" s="12"/>
       <c r="P37" s="12">
@@ -17618,18 +17666,18 @@
       </c>
       <c r="Q37" s="12"/>
       <c r="R37" s="12">
-        <v>8118000</v>
+        <v>1350000</v>
       </c>
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12">
-        <v>2772000</v>
+        <v>1207500</v>
       </c>
       <c r="V37" s="12"/>
     </row>
     <row r="38" ht="13.50" customHeight="1" outlineLevel="0">
       <c r="A38" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -17638,10 +17686,10 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="I38" s="12">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J38" s="12">
-        <v>180000</v>
+        <v>300000</v>
       </c>
       <c r="K38" s="12"/>
       <c r="P38" s="12">
@@ -17649,106 +17697,571 @@
       </c>
       <c r="Q38" s="12"/>
       <c r="R38" s="12">
-        <v>180000</v>
+        <v>300000</v>
       </c>
       <c r="S38" s="12"/>
       <c r="T38" s="12"/>
       <c r="U38" s="12">
-        <v>75600</v>
+        <v>189000</v>
       </c>
       <c r="V38" s="12"/>
     </row>
     <row r="39" ht="13.50" customHeight="1" outlineLevel="0">
-      <c r="C39" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="I39" s="14">
-        <v>668</v>
-      </c>
-      <c r="J39" s="14">
-        <v>28016000</v>
-      </c>
-      <c r="K39" s="14"/>
-      <c r="P39" s="14">
+      <c r="A39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="I39" s="12">
+        <v>9</v>
+      </c>
+      <c r="J39" s="12">
+        <v>162000</v>
+      </c>
+      <c r="K39" s="12"/>
+      <c r="P39" s="12">
         <v>0</v>
       </c>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14">
-        <v>28016000</v>
-      </c>
-      <c r="S39" s="14"/>
-      <c r="T39" s="14"/>
-      <c r="U39" s="14">
-        <v>10407600</v>
-      </c>
-      <c r="V39" s="14"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12">
+        <v>162000</v>
+      </c>
+      <c r="S39" s="12"/>
+      <c r="T39" s="12"/>
+      <c r="U39" s="12">
+        <v>132300</v>
+      </c>
+      <c r="V39" s="12"/>
     </row>
-    <row r="40" ht="12.75" customHeight="1" outlineLevel="0"/>
-    <row r="41" ht="12.00" customHeight="1" outlineLevel="0"/>
+    <row r="40" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="I40" s="12">
+        <v>1</v>
+      </c>
+      <c r="J40" s="12">
+        <v>20000</v>
+      </c>
+      <c r="K40" s="12"/>
+      <c r="P40" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12">
+        <v>20000</v>
+      </c>
+      <c r="S40" s="12"/>
+      <c r="T40" s="12"/>
+      <c r="U40" s="12">
+        <v>12600</v>
+      </c>
+      <c r="V40" s="12"/>
+    </row>
+    <row r="41" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A41" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="I41" s="12">
+        <v>1</v>
+      </c>
+      <c r="J41" s="12">
+        <v>40000</v>
+      </c>
+      <c r="K41" s="12"/>
+      <c r="P41" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12">
+        <v>40000</v>
+      </c>
+      <c r="S41" s="12"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="12">
+        <v>25200</v>
+      </c>
+      <c r="V41" s="12"/>
+    </row>
     <row r="42" ht="13.50" customHeight="1" outlineLevel="0">
-      <c r="C42" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="I42" s="14">
-        <v>1383</v>
-      </c>
-      <c r="J42" s="14">
-        <v>49796000</v>
-      </c>
-      <c r="K42" s="14"/>
-      <c r="P42" s="14">
-        <v>813000</v>
-      </c>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14">
-        <v>48983000</v>
-      </c>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="14">
-        <v>10407600</v>
-      </c>
-      <c r="V42" s="14"/>
+      <c r="A42" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="I42" s="12">
+        <v>8</v>
+      </c>
+      <c r="J42" s="12">
+        <v>320000</v>
+      </c>
+      <c r="K42" s="12"/>
+      <c r="P42" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12">
+        <v>320000</v>
+      </c>
+      <c r="S42" s="12"/>
+      <c r="T42" s="12"/>
+      <c r="U42" s="12">
+        <v>201600</v>
+      </c>
+      <c r="V42" s="12"/>
     </row>
-    <row r="43" ht="12.75" customHeight="1" outlineLevel="0"/>
-    <row r="44" ht="273.75" customHeight="1" outlineLevel="0"/>
-    <row r="45" ht="42.00" customHeight="1" outlineLevel="0"/>
-    <row r="46" ht="15.75" customHeight="1" outlineLevel="0">
-      <c r="A46" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="15"/>
-      <c r="S46" s="15"/>
-      <c r="T46" s="15"/>
-      <c r="U46" s="15"/>
-      <c r="V46" s="15"/>
+    <row r="43" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="I43" s="12">
+        <v>10</v>
+      </c>
+      <c r="J43" s="12">
+        <v>380000</v>
+      </c>
+      <c r="K43" s="12"/>
+      <c r="P43" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="12">
+        <v>380000</v>
+      </c>
+      <c r="S43" s="12"/>
+      <c r="T43" s="12"/>
+      <c r="U43" s="12">
+        <v>266000</v>
+      </c>
+      <c r="V43" s="12"/>
+    </row>
+    <row r="44" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="I44" s="12">
+        <v>8</v>
+      </c>
+      <c r="J44" s="12">
+        <v>304000</v>
+      </c>
+      <c r="K44" s="12"/>
+      <c r="P44" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12">
+        <v>304000</v>
+      </c>
+      <c r="S44" s="12"/>
+      <c r="T44" s="12"/>
+      <c r="U44" s="12">
+        <v>212800</v>
+      </c>
+      <c r="V44" s="12"/>
+    </row>
+    <row r="45" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="I45" s="12">
+        <v>12</v>
+      </c>
+      <c r="J45" s="12">
+        <v>480000</v>
+      </c>
+      <c r="K45" s="12"/>
+      <c r="P45" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12">
+        <v>480000</v>
+      </c>
+      <c r="S45" s="12"/>
+      <c r="T45" s="12"/>
+      <c r="U45" s="12">
+        <v>302400</v>
+      </c>
+      <c r="V45" s="12"/>
+    </row>
+    <row r="46" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="I46" s="12">
+        <v>6</v>
+      </c>
+      <c r="J46" s="12">
+        <v>228000</v>
+      </c>
+      <c r="K46" s="12"/>
+      <c r="P46" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12">
+        <v>228000</v>
+      </c>
+      <c r="S46" s="12"/>
+      <c r="T46" s="12"/>
+      <c r="U46" s="12">
+        <v>159600</v>
+      </c>
+      <c r="V46" s="12"/>
+    </row>
+    <row r="47" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="I47" s="12">
+        <v>56</v>
+      </c>
+      <c r="J47" s="12">
+        <v>1456000</v>
+      </c>
+      <c r="K47" s="12"/>
+      <c r="P47" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12">
+        <v>1456000</v>
+      </c>
+      <c r="S47" s="12"/>
+      <c r="T47" s="12"/>
+      <c r="U47" s="12">
+        <v>2156000</v>
+      </c>
+      <c r="V47" s="12"/>
+    </row>
+    <row r="48" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="I48" s="12">
+        <v>1</v>
+      </c>
+      <c r="J48" s="12">
+        <v>28000</v>
+      </c>
+      <c r="K48" s="12"/>
+      <c r="P48" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12">
+        <v>28000</v>
+      </c>
+      <c r="S48" s="12"/>
+      <c r="T48" s="12"/>
+      <c r="U48" s="12">
+        <v>36400</v>
+      </c>
+      <c r="V48" s="12"/>
+    </row>
+    <row r="49" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A49" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="I49" s="12">
+        <v>14</v>
+      </c>
+      <c r="J49" s="12">
+        <v>392000</v>
+      </c>
+      <c r="K49" s="12"/>
+      <c r="P49" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12">
+        <v>392000</v>
+      </c>
+      <c r="S49" s="12"/>
+      <c r="T49" s="12"/>
+      <c r="U49" s="12">
+        <v>509600</v>
+      </c>
+      <c r="V49" s="12"/>
+    </row>
+    <row r="50" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A50" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="I50" s="12">
+        <v>7</v>
+      </c>
+      <c r="J50" s="12">
+        <v>196000</v>
+      </c>
+      <c r="K50" s="12"/>
+      <c r="P50" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12">
+        <v>196000</v>
+      </c>
+      <c r="S50" s="12"/>
+      <c r="T50" s="12"/>
+      <c r="U50" s="12">
+        <v>254800</v>
+      </c>
+      <c r="V50" s="12"/>
+    </row>
+    <row r="51" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A51" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="I51" s="12">
+        <v>1</v>
+      </c>
+      <c r="J51" s="12">
+        <v>28000</v>
+      </c>
+      <c r="K51" s="12"/>
+      <c r="P51" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12">
+        <v>28000</v>
+      </c>
+      <c r="S51" s="12"/>
+      <c r="T51" s="12"/>
+      <c r="U51" s="12">
+        <v>36400</v>
+      </c>
+      <c r="V51" s="12"/>
+    </row>
+    <row r="52" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A52" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="I52" s="12">
+        <v>80</v>
+      </c>
+      <c r="J52" s="12">
+        <v>400000</v>
+      </c>
+      <c r="K52" s="12"/>
+      <c r="P52" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12">
+        <v>400000</v>
+      </c>
+      <c r="S52" s="12"/>
+      <c r="T52" s="12"/>
+      <c r="U52" s="12">
+        <v>392000</v>
+      </c>
+      <c r="V52" s="12"/>
+    </row>
+    <row r="53" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="A53" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="I53" s="12">
+        <v>60</v>
+      </c>
+      <c r="J53" s="12">
+        <v>0</v>
+      </c>
+      <c r="K53" s="12"/>
+      <c r="P53" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12">
+        <v>0</v>
+      </c>
+      <c r="S53" s="12"/>
+      <c r="T53" s="12"/>
+      <c r="U53" s="12">
+        <v>2982000</v>
+      </c>
+      <c r="V53" s="12"/>
+    </row>
+    <row r="54" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="C54" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="I54" s="14">
+        <v>721</v>
+      </c>
+      <c r="J54" s="14">
+        <v>24175000</v>
+      </c>
+      <c r="K54" s="14"/>
+      <c r="P54" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14">
+        <v>24175000</v>
+      </c>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="14">
+        <v>11633300</v>
+      </c>
+      <c r="V54" s="14"/>
+    </row>
+    <row r="55" ht="12.75" customHeight="1" outlineLevel="0"/>
+    <row r="56" ht="12.00" customHeight="1" outlineLevel="0"/>
+    <row r="57" ht="13.50" customHeight="1" outlineLevel="0">
+      <c r="C57" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="I57" s="14">
+        <v>964</v>
+      </c>
+      <c r="J57" s="14">
+        <v>29035000</v>
+      </c>
+      <c r="K57" s="14"/>
+      <c r="P57" s="14">
+        <v>267300</v>
+      </c>
+      <c r="Q57" s="14"/>
+      <c r="R57" s="14">
+        <v>28767700</v>
+      </c>
+      <c r="S57" s="14"/>
+      <c r="T57" s="14"/>
+      <c r="U57" s="14">
+        <v>11633300</v>
+      </c>
+      <c r="V57" s="14"/>
+    </row>
+    <row r="58" ht="12.75" customHeight="1" outlineLevel="0"/>
+    <row r="59" ht="93.75" customHeight="1" outlineLevel="0"/>
+    <row r="60" ht="42.00" customHeight="1" outlineLevel="0"/>
+    <row r="61" ht="15.75" customHeight="1" outlineLevel="0">
+      <c r="A61" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="15"/>
+      <c r="S61" s="15"/>
+      <c r="T61" s="15"/>
+      <c r="U61" s="15"/>
+      <c r="V61" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="129">
+  <mergeCells count="204">
     <mergeCell ref="A2:V2"/>
     <mergeCell ref="A3:V3"/>
     <mergeCell ref="B5:C5"/>
@@ -17780,33 +18293,33 @@
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="U16:V16"/>
-    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="C17:G17"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="P17:Q17"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="U17:V17"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="A21:V21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="A23:G24"/>
-    <mergeCell ref="J23:K24"/>
-    <mergeCell ref="P23:Q24"/>
-    <mergeCell ref="R23:T24"/>
-    <mergeCell ref="U23:V24"/>
+    <mergeCell ref="A19:V19"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="A21:G22"/>
+    <mergeCell ref="J21:K22"/>
+    <mergeCell ref="P21:Q22"/>
+    <mergeCell ref="R21:T22"/>
+    <mergeCell ref="U21:V22"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="U23:V23"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="J25:K25"/>
     <mergeCell ref="P25:Q25"/>
     <mergeCell ref="R25:T25"/>
     <mergeCell ref="U25:V25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="U26:V26"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="J27:K27"/>
     <mergeCell ref="P27:Q27"/>
@@ -17867,17 +18380,92 @@
     <mergeCell ref="P38:Q38"/>
     <mergeCell ref="R38:T38"/>
     <mergeCell ref="U38:V38"/>
-    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="A39:G39"/>
     <mergeCell ref="J39:K39"/>
     <mergeCell ref="P39:Q39"/>
     <mergeCell ref="R39:T39"/>
     <mergeCell ref="U39:V39"/>
-    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="R40:T40"/>
+    <mergeCell ref="U40:V40"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="R41:T41"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="A42:G42"/>
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="P42:Q42"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="U42:V42"/>
-    <mergeCell ref="A46:V46"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="U43:V43"/>
+    <mergeCell ref="A44:G44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="U44:V44"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="P45:Q45"/>
+    <mergeCell ref="R45:T45"/>
+    <mergeCell ref="U45:V45"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="R46:T46"/>
+    <mergeCell ref="U46:V46"/>
+    <mergeCell ref="A47:G47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="R47:T47"/>
+    <mergeCell ref="U47:V47"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="R48:T48"/>
+    <mergeCell ref="U48:V48"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="R49:T49"/>
+    <mergeCell ref="U49:V49"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="P50:Q50"/>
+    <mergeCell ref="R50:T50"/>
+    <mergeCell ref="U50:V50"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="P51:Q51"/>
+    <mergeCell ref="R51:T51"/>
+    <mergeCell ref="U51:V51"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="P52:Q52"/>
+    <mergeCell ref="R52:T52"/>
+    <mergeCell ref="U52:V52"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="P53:Q53"/>
+    <mergeCell ref="R53:T53"/>
+    <mergeCell ref="U53:V53"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="R54:T54"/>
+    <mergeCell ref="U54:V54"/>
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="R57:T57"/>
+    <mergeCell ref="U57:V57"/>
+    <mergeCell ref="A61:V61"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>